<commit_message>
User: handle can complete grade twelve
</commit_message>
<xml_diff>
--- a/db/csv/self_understanding_question.xlsx
+++ b/db/csv/self_understanding_question.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
   <si>
     <t>code</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>score</t>
   </si>
   <si>
     <t>q1_o1</t>
@@ -640,19 +643,25 @@
       <c r="D1" s="4" t="s">
         <v>24</v>
       </c>
+      <c r="E1" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
@@ -660,13 +669,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="4">
@@ -674,13 +686,16 @@
         <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
@@ -688,13 +703,16 @@
         <v>7</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -702,13 +720,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="7">
@@ -716,13 +737,16 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
@@ -730,13 +754,16 @@
         <v>12</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.0</v>
       </c>
     </row>
     <row r="9">
@@ -744,13 +771,16 @@
         <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
@@ -758,13 +788,16 @@
         <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.0</v>
       </c>
     </row>
     <row r="11">
@@ -772,13 +805,16 @@
         <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -786,13 +822,16 @@
         <v>17</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.0</v>
       </c>
     </row>
     <row r="13">
@@ -800,13 +839,13 @@
         <v>19</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14">
@@ -814,13 +853,13 @@
         <v>19</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
@@ -828,13 +867,13 @@
         <v>19</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16">
@@ -842,13 +881,13 @@
         <v>19</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17">
@@ -856,13 +895,13 @@
         <v>19</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18">
@@ -870,13 +909,13 @@
         <v>19</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>